<commit_message>
Added a retry scope on the Navigate Activity - Search_by_Username.xaml
</commit_message>
<xml_diff>
--- a/Data/messages.xlsx
+++ b/Data/messages.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B0C924-430A-4048-B0DB-C7C657051F3D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7BB38C-0FB6-437A-BDEF-69A0F2C2E478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,36 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Hi bro, bot test2</t>
-  </si>
-  <si>
-    <t>Hi bro, bot test3</t>
-  </si>
-  <si>
-    <t>Hi bro, bot test4</t>
-  </si>
-  <si>
-    <t>Hi bro, bot test5</t>
-  </si>
-  <si>
-    <t>Hi bro, bot test6</t>
-  </si>
-  <si>
-    <t>Hi bro, bot test7</t>
-  </si>
-  <si>
-    <t>Hi bro, bot test8</t>
-  </si>
-  <si>
-    <t>Hi bro, bot test9</t>
-  </si>
-  <si>
-    <t>Hi bro, bot test1</t>
-  </si>
-  <si>
-    <t>Hi bro, bot test10</t>
+    <t>Hi bro, bot test</t>
   </si>
 </sst>
 </file>
@@ -367,10 +340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,52 +353,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>